<commit_message>
N-CTU delete JP command
</commit_message>
<xml_diff>
--- a/build-N-XTU-Desktop_Qt_5_8_0_MinGW_32bit-Debug/2018-10-29.xlsx
+++ b/build-N-XTU-Desktop_Qt_5_8_0_MinGW_32bit-Debug/2018-10-29.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>STATUS</t>
   </si>
@@ -55,45 +55,13 @@
   </si>
   <si>
     <t>TIME</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>000B57FFFEF609E6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>122.834 mA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20.002 mA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0.012 mA</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>OK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0015</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="176" formatCode="0.0%"/>
-    <numFmt numFmtId="177" formatCode="yyyy/mm/dd\ hh:mm:ss"/>
-  </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,22 +83,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -157,7 +109,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -169,18 +121,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -476,24 +416,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M2"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.25" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="4.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.5" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="3" customFormat="1">
@@ -535,47 +474,6 @@
       </c>
       <c r="M1" s="2" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="4">
-        <v>-46</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="4">
-        <v>-46</v>
-      </c>
-      <c r="F2" s="6">
-        <v>1</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" s="7">
-        <v>43402.469282407408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>